<commit_message>
Many changes done. Caching removed and makes individual service for each category
</commit_message>
<xml_diff>
--- a/src/main/resources/nxData_local.xlsx
+++ b/src/main/resources/nxData_local.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MunishData\mp\project\workspace\shop\shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{963C15B0-BBE1-4EC4-A173-6C4CB857F425}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B738615D-7A5F-460B-9F2C-A38CDF037BB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
   </bookViews>
@@ -21,6 +21,8 @@
     <sheet name="ChemistsListing" sheetId="9" r:id="rId6"/>
     <sheet name="SchoolsListing" sheetId="5" r:id="rId7"/>
     <sheet name="PlaySchoolsListing" sheetId="8" r:id="rId8"/>
+    <sheet name="AutomobilesListing" sheetId="10" r:id="rId9"/>
+    <sheet name="ShoppingListing" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="357">
   <si>
     <t>RESTAURANTS</t>
   </si>
@@ -1049,6 +1051,60 @@
   </si>
   <si>
     <t>Jagat Pramukh Market</t>
+  </si>
+  <si>
+    <t>Ncr Wheels, Apna Garage</t>
+  </si>
+  <si>
+    <t>Village Iteda, Iteda Gol Chakkar, Near Gaur Saundaryam 130 mtr Road, Opp. Eco Village-II, Greater Noida West (Noida Extension)</t>
+  </si>
+  <si>
+    <t>09999441148</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>09:30AM to 08:00PM</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?tbm=lcl&amp;ei=9LPKXJ3sPKndz7sPluuBmA0&amp;q=ncrwheels+gretaer+noida&amp;oq=ncrwheels+gretaer+noida&amp;gs_l=psy-ab.3..33i21k1j33i160k1.9745.11690.0.11739.13.9.0.0.0.0.333.885.2-2j1.3.0....0...1c.1.64.psy-ab..10.3.885....0.rSpGw2fYmJ0#rlfi=hd:;si:;mv:!1m2!1d28.606900277319028!2d77.43943090264295!2m2!1d28.60654032268097!2d77.43902089735704</t>
+  </si>
+  <si>
+    <t>/img/automobiles/automobiles_NcrWheelsApnaGarage.jpeg</t>
+  </si>
+  <si>
+    <t>Bedsheets &amp; Bags</t>
+  </si>
+  <si>
+    <t>Y-4, 604, Eros Sampoornam, Sector 2, Plot No GH-01, Greater Noida West (Noida Extension)</t>
+  </si>
+  <si>
+    <t>09560929494, 09910554248</t>
+  </si>
+  <si>
+    <t>10:00AM to 05:00PM</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?tbm=lcl&amp;ei=1sXKXKKQFMKH9QOV3oiYBQ&amp;q=eros+sampoornam+noida+extension&amp;oq=Eros.+Sampoornam&amp;gs_l=psy-ab.1.1.0i22i30k1l10.9859807.9859807.0.9861546.1.1.0.0.0.0.322.322.3-1.1.0....0...1c..64.psy-ab..0.1.322....0.sOA2aj3mwV4#rlfi=hd:;si:5673722420266658090;mv:!1m2!1d28.58985197731903!2d77.45860386939077!2m2!1d28.58949202268097!2d77.45819393060923</t>
+  </si>
+  <si>
+    <t>Eros Sampoornam</t>
+  </si>
+  <si>
+    <t>/img/shopping/shopping_BedsheetsBags.jpeg</t>
+  </si>
+  <si>
+    <t>SHOPPING</t>
+  </si>
+  <si>
+    <t>EVENTS</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>MOVIES</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1127,6 +1183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1441,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226CACE2-D48A-4B7A-816A-2A1EDF39A2C2}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1489,86 +1546,187 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>354</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F7B1AF-7472-40BE-942A-443ED2CD4998}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1577,7 +1735,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1692,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736B90CF-4517-4B11-8606-27B03FD2621D}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2041,9 +2199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E0A812-8013-4DA9-80BD-D58FA7A436A2}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2723,9 +2879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6312478D-59AA-47FA-A2EB-CCE0DB7145BD}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2988,9 +3142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D053C47-CCAB-4F6A-B908-C30E1288A5C4}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3107,9 +3259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B005557-25B7-4487-BE06-E764B2181BB1}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3316,9 +3466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6DBBAB-95B6-43EE-9DCA-B017464EB0E9}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3410,4 +3558,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671CDC17-D331-4018-9460-7F7B401CEC28}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="164.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added news and other
</commit_message>
<xml_diff>
--- a/src/main/resources/nxData_local.xlsx
+++ b/src/main/resources/nxData_local.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MunishData\mp\project\workspace\shop\shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B738615D-7A5F-460B-9F2C-A38CDF037BB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4289A5EF-A9E2-4752-BD6D-2D0011EDE6F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Category" sheetId="3" r:id="rId1"/>
-    <sheet name="CategoryThumbnail" sheetId="2" r:id="rId2"/>
-    <sheet name="RestaurantsListing" sheetId="1" r:id="rId3"/>
-    <sheet name="DoctorsListing" sheetId="7" r:id="rId4"/>
-    <sheet name="HospitalsListing" sheetId="4" r:id="rId5"/>
-    <sheet name="ChemistsListing" sheetId="9" r:id="rId6"/>
-    <sheet name="SchoolsListing" sheetId="5" r:id="rId7"/>
-    <sheet name="PlaySchoolsListing" sheetId="8" r:id="rId8"/>
-    <sheet name="AutomobilesListing" sheetId="10" r:id="rId9"/>
-    <sheet name="ShoppingListing" sheetId="11" r:id="rId10"/>
+    <sheet name="NewsList" sheetId="12" r:id="rId1"/>
+    <sheet name="Category" sheetId="3" r:id="rId2"/>
+    <sheet name="CategoryThumbnail" sheetId="2" r:id="rId3"/>
+    <sheet name="RestaurantsListing" sheetId="1" r:id="rId4"/>
+    <sheet name="DoctorsListing" sheetId="7" r:id="rId5"/>
+    <sheet name="HospitalsListing" sheetId="4" r:id="rId6"/>
+    <sheet name="ChemistsListing" sheetId="9" r:id="rId7"/>
+    <sheet name="SchoolsListing" sheetId="5" r:id="rId8"/>
+    <sheet name="PlaySchoolsListing" sheetId="8" r:id="rId9"/>
+    <sheet name="AutomobilesListing" sheetId="10" r:id="rId10"/>
+    <sheet name="ShoppingListing" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="361">
   <si>
     <t>RESTAURANTS</t>
   </si>
@@ -1105,6 +1106,18 @@
   </si>
   <si>
     <t>MOVIES</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>newsURL</t>
+  </si>
+  <si>
+    <t>Complaints by home buyers on rise, UP-RERA opens third bench in Noida</t>
+  </si>
+  <si>
+    <t>https://economictimes.indiatimes.com/wealth/personal-finance-news/complaints-by-home-buyers-on-rise-up-rera-opens-third-bench-in-noida/articleshow/69038470.cms</t>
   </si>
 </sst>
 </file>
@@ -1497,163 +1510,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226CACE2-D48A-4B7A-816A-2A1EDF39A2C2}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD1AE64-8B0F-4628-88A7-5C972E1E7661}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="146.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>357</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>76</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>354</v>
-      </c>
-      <c r="B11" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>353</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>356</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>359</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671CDC17-D331-4018-9460-7F7B401CEC28}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="164.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H2" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F7B1AF-7472-40BE-942A-443ED2CD4998}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1731,6 +1696,163 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{226CACE2-D48A-4B7A-816A-2A1EDF39A2C2}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>354</v>
+      </c>
+      <c r="B11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F0836F-3908-4833-B8F0-93FF494A7A6F}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -1846,7 +1968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736B90CF-4517-4B11-8606-27B03FD2621D}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -2195,7 +2317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E0A812-8013-4DA9-80BD-D58FA7A436A2}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -2875,7 +2997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6312478D-59AA-47FA-A2EB-CCE0DB7145BD}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -3138,7 +3260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D053C47-CCAB-4F6A-B908-C30E1288A5C4}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -3255,7 +3377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B005557-25B7-4487-BE06-E764B2181BB1}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -3462,7 +3584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6DBBAB-95B6-43EE-9DCA-B017464EB0E9}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -3558,79 +3680,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671CDC17-D331-4018-9460-7F7B401CEC28}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="164.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>342</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>343</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H2" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
daily needs jsp added
</commit_message>
<xml_diff>
--- a/src/main/resources/nxData_local.xlsx
+++ b/src/main/resources/nxData_local.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MunishData\mp\project\workspace\shop\shop\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B62BE429-0C05-459E-A43B-BCE7CE272FA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60353E3-3FE8-48E9-9AF1-612491B74E9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" firstSheet="7" activeTab="11" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" firstSheet="10" activeTab="12" xr2:uid="{4A692815-A8AB-4C25-93C4-DEA366F4764C}"/>
   </bookViews>
   <sheets>
     <sheet name="NewsList" sheetId="12" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="ShoppingListing" sheetId="11" r:id="rId10"/>
     <sheet name="PharmacyListing" sheetId="15" r:id="rId11"/>
     <sheet name="PathLabsListing" sheetId="16" r:id="rId12"/>
+    <sheet name="DailyNeedsListing" sheetId="18" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="667">
   <si>
     <t>RESTAURANTS</t>
   </si>
@@ -1977,6 +1978,66 @@
   </si>
   <si>
     <t>Life Care Pathology Lab</t>
+  </si>
+  <si>
+    <t>Family Store</t>
+  </si>
+  <si>
+    <t>LGF 41, City Plaza, Gaur City, Greater Noida West (Noida Extension)</t>
+  </si>
+  <si>
+    <t>09599975791, 09599975792, 07827439297</t>
+  </si>
+  <si>
+    <t>/img/dailyNeeds/dailyNeeds_FamilyStore.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Family+Store/@28.6146087,77.4255353,17z/data=!3m1!4b1!4m5!3m4!1s0x390cee4b8783e553:0x652d6c4956ab52f6!8m2!3d28.614604!4d77.427724</t>
+  </si>
+  <si>
+    <t>City Plaza, Gaur City</t>
+  </si>
+  <si>
+    <t>Mini Mart</t>
+  </si>
+  <si>
+    <t>Shop no.23, City plaza, Gaur city 1, Greater Noida West (Noida Extension)</t>
+  </si>
+  <si>
+    <t>08800563608</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.Minimart.com </t>
+  </si>
+  <si>
+    <t>08:00AM to 09:30PM</t>
+  </si>
+  <si>
+    <t>/img/dailyNeeds/dailyNeeds_MiniMart.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Mini+Mart/@28.6150307,77.4255613,17z/data=!3m1!4b1!4m5!3m4!1s0x390cee4b85c7e24d:0x984467dc816981a0!8m2!3d28.615026!4d77.42775</t>
+  </si>
+  <si>
+    <t>One Stop Mart</t>
+  </si>
+  <si>
+    <t>Shop Number 45-50, Lower Ground Floor, Galliria Market, Gaur City 2, Greater Noida West (Noida Extension)</t>
+  </si>
+  <si>
+    <t>07290016382, 07290016383</t>
+  </si>
+  <si>
+    <t>24 Hrs</t>
+  </si>
+  <si>
+    <t>/img/dailyNeeds/dailyNeeds_OneStopMart.jpeg</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/One+Stop+Mart/@28.619435,77.4210851,17z/data=!3m1!4b1!4m5!3m4!1s0x390cefb559f85485:0x6e99725b0e217cc2!8m2!3d28.6194303!4d77.4232738</t>
+  </si>
+  <si>
+    <t>Galliria Market, Gaur City</t>
   </si>
 </sst>
 </file>
@@ -3936,7 +3997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7299E0-EDDE-4C29-B4A5-17E466E21EB2}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4592,6 +4653,199 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A70DA5-FDBE-4DF0-8E73-709D711D459B}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="61.6328125" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>647</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>648</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>649</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>650</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="K2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>653</v>
+      </c>
+      <c r="E3" t="s">
+        <v>654</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>655</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>657</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="J3" t="s">
+        <v>659</v>
+      </c>
+      <c r="K3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>660</v>
+      </c>
+      <c r="E4" t="s">
+        <v>661</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>663</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="J4" t="s">
+        <v>665</v>
+      </c>
+      <c r="K4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="F11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>